<commit_message>
US Mexican import prices and quantities added
</commit_message>
<xml_diff>
--- a/Price_Study/Spain/Plots/Summary_Blueberry.xlsx
+++ b/Price_Study/Spain/Plots/Summary_Blueberry.xlsx
@@ -435,10 +435,10 @@
         <v>3.306672764223181</v>
       </c>
       <c r="E2">
-        <v>3.539005115574545</v>
+        <v>3.682053159252038</v>
       </c>
       <c r="F2">
-        <v>6.404999999999999</v>
+        <v>5.41</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -455,10 +455,10 @@
         <v>5.380240645152319</v>
       </c>
       <c r="E3">
-        <v>5.245735854262728</v>
+        <v>5.965051755218097</v>
       </c>
       <c r="F3">
-        <v>6.71</v>
+        <v>6.385616604281449</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -475,10 +475,10 @@
         <v>7.730711008615206</v>
       </c>
       <c r="E4">
-        <v>7.143040392967862</v>
+        <v>7.115699172182123</v>
       </c>
       <c r="F4">
-        <v>6.954999999999999</v>
+        <v>6.705381561317198</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -495,10 +495,10 @@
         <v>23</v>
       </c>
       <c r="E5">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -518,7 +518,7 @@
         <v>7.890560994867744</v>
       </c>
       <c r="F6">
-        <v>7.21</v>
+        <v>7.313857748729716</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -535,10 +535,10 @@
         <v>5.593250257518018</v>
       </c>
       <c r="E7">
-        <v>5.232148635520834</v>
+        <v>5.306426188541749</v>
       </c>
       <c r="F7">
-        <v>6.665714285714285</v>
+        <v>5.981500086660821</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -558,7 +558,7 @@
         <v>2.227396371871529</v>
       </c>
       <c r="F8">
-        <v>6.02</v>
+        <v>3.56</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -575,10 +575,10 @@
         <v>2.219988614151075</v>
       </c>
       <c r="E9">
-        <v>1.988241591266751</v>
+        <v>1.981494588585559</v>
       </c>
       <c r="F9">
-        <v>0.414522100048443</v>
+        <v>1.104760956810323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
USMX prices unified in single notebook and ES prices fixed
</commit_message>
<xml_diff>
--- a/Price_Study/Spain/Plots/Summary_Blueberry.xlsx
+++ b/Price_Study/Spain/Plots/Summary_Blueberry.xlsx
@@ -438,7 +438,7 @@
         <v>3.682053159252038</v>
       </c>
       <c r="F2">
-        <v>5.41</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -458,7 +458,7 @@
         <v>5.965051755218097</v>
       </c>
       <c r="F3">
-        <v>6.385616604281449</v>
+        <v>6.119378603558825</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -478,7 +478,7 @@
         <v>7.115699172182123</v>
       </c>
       <c r="F4">
-        <v>6.705381561317198</v>
+        <v>6.682026959004283</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -498,7 +498,7 @@
         <v>25</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -538,7 +538,7 @@
         <v>5.306426188541749</v>
       </c>
       <c r="F7">
-        <v>5.981500086660821</v>
+        <v>5.68775654336231</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -558,7 +558,7 @@
         <v>2.227396371871529</v>
       </c>
       <c r="F8">
-        <v>3.56</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -578,7 +578,7 @@
         <v>1.981494588585559</v>
       </c>
       <c r="F9">
-        <v>1.104760956810323</v>
+        <v>1.35705221483896</v>
       </c>
     </row>
   </sheetData>

</xml_diff>